<commit_message>
Atualizando arquivos e implementação dos agentes
</commit_message>
<xml_diff>
--- a/planilha tcc.xlsx
+++ b/planilha tcc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="0" windowWidth="19560" windowHeight="9630"/>
+    <workbookView xWindow="12090" yWindow="0" windowWidth="19560" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Entrega 01" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>Título do projeto:</t>
   </si>
@@ -104,6 +104,42 @@
   </si>
   <si>
     <t>criar indexcss</t>
+  </si>
+  <si>
+    <t>Sem nenhum problemas até o momento</t>
+  </si>
+  <si>
+    <t>Modificação no banco de dados</t>
+  </si>
+  <si>
+    <t>Já upados</t>
+  </si>
+  <si>
+    <t>criar login_agente</t>
+  </si>
+  <si>
+    <t>criar verificação_agente</t>
+  </si>
+  <si>
+    <t>criar home_agente</t>
+  </si>
+  <si>
+    <t>criar menu_agente</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>adicionar informações no banco</t>
+  </si>
+  <si>
+    <t>cria_pagina_noticia</t>
+  </si>
+  <si>
+    <t>adicionar_vacinas</t>
+  </si>
+  <si>
+    <t>criar_pagina_doses_vacina</t>
   </si>
 </sst>
 </file>
@@ -202,7 +238,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -221,9 +257,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -480,8 +513,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -496,23 +529,23 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -551,7 +584,9 @@
       <c r="D5" s="5">
         <v>44346</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
@@ -563,13 +598,15 @@
       <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>44346</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>44345</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -578,13 +615,15 @@
       <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>44346</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>44345</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -593,44 +632,50 @@
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>44346</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="7">
         <v>44348</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>44348</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>44348</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -643,15 +688,17 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -661,7 +708,7 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="2"/>
@@ -687,73 +734,113 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>44351</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
+      <c r="C17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="7">
+        <v>44358</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
+      <c r="A18" s="7">
+        <v>44351</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="7">
+        <v>44358</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
+      <c r="A19" s="7">
         <v>44351</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="9"/>
+      <c r="C19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="7">
+        <v>44358</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>44351</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="10"/>
+      <c r="C20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="7">
+        <v>44358</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="8">
+      <c r="A21" s="7">
         <v>44351</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
+      <c r="C21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="7">
+        <v>44358</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="8">
-        <v>44351</v>
+      <c r="A22" s="7">
+        <v>44354</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="C22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="7">
+        <v>44358</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="9"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
@@ -763,7 +850,7 @@
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="6"/>
@@ -789,43 +876,89 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="7">
+        <v>44371</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
+      <c r="C27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="7">
+        <v>44375</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
+      <c r="A28" s="7">
+        <v>44371</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="7">
+        <v>44375</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
+      <c r="A29" s="7">
+        <v>44371</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="7">
+        <v>44375</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="10"/>
+      <c r="A30" s="7">
+        <v>44371</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="7">
+        <v>44375</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="9"/>
+      <c r="A31" s="7">
+        <v>44371</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="7">
+        <v>44375</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
@@ -835,53 +968,75 @@
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="A33" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="A34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="8"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="8"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>

</xml_diff>

<commit_message>
Adicionamos alguns arquivos de local, agendamento e alteramos o banco, iremos complementar com o 5 sprint caso tenha ficado estranho (pois dividimos em dois sprints complementares)
</commit_message>
<xml_diff>
--- a/planilha tcc.xlsx
+++ b/planilha tcc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12090" yWindow="0" windowWidth="19560" windowHeight="9630"/>
+    <workbookView xWindow="16740" yWindow="0" windowWidth="19560" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Entrega 01" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
   <si>
     <t>Título do projeto:</t>
   </si>
@@ -133,13 +133,70 @@
     <t>adicionar informações no banco</t>
   </si>
   <si>
-    <t>cria_pagina_noticia</t>
+    <t>Sem nenhum problemas até o momento, na real deu um pequeno erro mas já foi solucionado.</t>
   </si>
   <si>
-    <t>adicionar_vacinas</t>
+    <t>decidimos não criar a pagina de noticias (pelo menos no momento)</t>
   </si>
   <si>
-    <t>criar_pagina_doses_vacina</t>
+    <t>concluído</t>
+  </si>
+  <si>
+    <t>tranquilo até o momento.</t>
+  </si>
+  <si>
+    <t>listar vacinas</t>
+  </si>
+  <si>
+    <t>adicionar vacinas</t>
+  </si>
+  <si>
+    <t>inserir vacina</t>
+  </si>
+  <si>
+    <t>criar vacinas</t>
+  </si>
+  <si>
+    <t>criar adm_vacina</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>adicionar remove_vacina</t>
+  </si>
+  <si>
+    <t>adicionar altera vacina</t>
+  </si>
+  <si>
+    <t>insere local</t>
+  </si>
+  <si>
+    <t>lista_local</t>
+  </si>
+  <si>
+    <t>altera_local</t>
+  </si>
+  <si>
+    <t>a fazer.</t>
+  </si>
+  <si>
+    <t>remove_local</t>
+  </si>
+  <si>
+    <t>criar doses</t>
+  </si>
+  <si>
+    <t>criar_agendamento</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tivemos um pequeno problema na hora de implementar as vacinas, porém, conseguimos resolver. </t>
+  </si>
+  <si>
+    <t>Havia dado um erro no banco, mas era por causa de um primary key. Mas já concertamos.</t>
   </si>
 </sst>
 </file>
@@ -238,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -292,6 +349,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -511,10 +574,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -906,7 +969,7 @@
         <v>44375</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -967,7 +1030,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
         <v>35</v>
       </c>
@@ -976,7 +1039,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
@@ -993,146 +1056,242 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
+        <v>44378</v>
+      </c>
       <c r="B35" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D35" s="7"/>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="7"/>
+      <c r="E35" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
+        <v>44387</v>
+      </c>
       <c r="B36" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D36" s="7"/>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="7"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
+        <v>44388</v>
+      </c>
       <c r="B37" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D37" s="7"/>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="7"/>
+      <c r="E37" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>44388</v>
+      </c>
       <c r="B38" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="6"/>
       <c r="D38" s="7"/>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="10"/>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>44380</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D39" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
+        <v>44381</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
+        <v>44388</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
+      <c r="E41" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
+        <v>44388</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" s="7"/>
+      <c r="B46" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" s="7"/>
+      <c r="B47" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="7"/>
+      <c r="B48" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
+      <c r="B51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
+      <c r="B52" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
+      <c r="C53" s="6"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
     </row>
@@ -7766,9 +7925,11 @@
       <c r="E1000" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="E41:G42"/>
+    <mergeCell ref="E35:G36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1"/>

</xml_diff>